<commit_message>
UML Server Landscape Overview
</commit_message>
<xml_diff>
--- a/cheatsheets/xlsx/formulas.xlsx
+++ b/cheatsheets/xlsx/formulas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>mean:</t>
   </si>
@@ -40,15 +40,50 @@
   <si>
     <t>sum data points: #</t>
   </si>
+  <si>
+    <t>other one</t>
+  </si>
+  <si>
+    <t>too much light</t>
+  </si>
+  <si>
+    <t>not enough light</t>
+  </si>
+  <si>
+    <t>external issue</t>
+  </si>
+  <si>
+    <t>not seen! external issue?</t>
+  </si>
+  <si>
+    <t>not seen!</t>
+  </si>
+  <si>
+    <t>seen: 44</t>
+  </si>
+  <si>
+    <t>seen: 40</t>
+  </si>
+  <si>
+    <t>seen: 42</t>
+  </si>
+  <si>
+    <t>seen: 37</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Agfa Rotis Sans Serif"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Agfa Rotis Sans Serif"/>
       <family val="2"/>
     </font>
@@ -73,7 +108,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -82,49 +117,22 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="5">
     <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -137,9 +145,11 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -183,7 +193,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="31750" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -192,15 +202,79 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -210,10 +284,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$A$1:$A$42</c:f>
+              <c:f>Tabelle1!$A$1:$A$80</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="80"/>
                 <c:pt idx="0">
                   <c:v>44222</c:v>
                 </c:pt>
@@ -339,16 +413,130 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>44263</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44264</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44265</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44266</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44267</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>44268</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>44269</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>44270</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>44271</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>44272</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>44273</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44274</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>44275</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>44276</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>44277</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>44278</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>44279</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>44280</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>44281</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>44282</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>44283</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>44284</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>44285</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>44286</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>44287</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>44288</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>44289</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>44290</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>44291</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>44292</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>44293</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>44294</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>44295</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>44296</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>44297</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>44298</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>44299</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>44300</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>44301</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$1:$B$42</c:f>
+              <c:f>Tabelle1!$B$1:$B$80</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="80"/>
                 <c:pt idx="0">
                   <c:v>44</c:v>
                 </c:pt>
@@ -383,6 +571,117 @@
                   <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="72">
                   <c:v>55</c:v>
                 </c:pt>
               </c:numCache>
@@ -396,13 +695,15 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="539351184"/>
         <c:axId val="539354136"/>
@@ -420,11 +721,11 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -436,11 +737,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -467,17 +768,29 @@
           <c:orientation val="minMax"/>
           <c:min val="30"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="95000"/>
+                      <a:lumOff val="5000"/>
+                      <a:alpha val="42000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                      <a:alpha val="36000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -487,33 +800,6 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="539351184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -531,14 +817,30 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="39000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="25000"/>
+          <a:lumOff val="75000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:round/>
@@ -604,146 +906,174 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="228">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+          <a:alpha val="75000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr"/>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr"/>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="31750" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -752,36 +1082,29 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="17"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -797,21 +1120,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -826,13 +1147,13 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -845,17 +1166,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -864,12 +1185,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -883,30 +1204,36 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -916,17 +1243,28 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -935,12 +1273,88 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="75000"/>
             <a:lumOff val="25000"/>
           </a:schemeClr>
@@ -948,64 +1362,6 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1013,14 +1369,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1032,12 +1388,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1046,14 +1402,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1062,9 +1417,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1082,9 +1437,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1095,11 +1450,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1107,14 +1467,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1124,15 +1478,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>171448</xdr:colOff>
+      <xdr:colOff>695325</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1417,101 +1771,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:K112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <pane xSplit="2" ySplit="28" topLeftCell="C62" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
+      <selection pane="bottomRight" activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="11" style="4"/>
-    <col min="4" max="4" width="17.875" customWidth="1"/>
+    <col min="3" max="3" width="11" style="6"/>
+    <col min="5" max="5" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="1">
         <v>44222</v>
       </c>
       <c r="B1" s="4">
         <v>44</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2">
+      <c r="F1" s="2">
         <f>AVERAGE(B:B)</f>
-        <v>51.5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>52.591836734693878</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>44223</v>
       </c>
       <c r="B2" s="4">
         <v>50</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <f>(COUNTIF(B:B,"&lt;55")/COUNT(B:B))*100</f>
-        <v>50</v>
-      </c>
-      <c r="F2" s="5"/>
-      <c r="J2">
+        <v>34.693877551020407</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="K2">
         <f>IF(B:B &lt; 55,1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>44224</v>
       </c>
       <c r="B3" s="4">
         <v>55</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <f>COUNT(B:B)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>44225</v>
       </c>
       <c r="B4" s="4">
         <v>55</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <f>COUNTIF(B:B,"&lt;55")</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>44226</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <f>COUNTIF(B:B,"&gt;54")</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>44227</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" s="1">
         <v>44228</v>
       </c>
@@ -1519,7 +1877,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
         <v>44229</v>
       </c>
@@ -1527,7 +1885,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" s="1">
         <v>44230</v>
       </c>
@@ -1535,7 +1893,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10" s="1">
         <v>44231</v>
       </c>
@@ -1543,7 +1901,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" s="1">
         <v>44232</v>
       </c>
@@ -1551,17 +1909,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11">
       <c r="A12" s="1">
         <v>44233</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11">
       <c r="A13" s="1">
         <v>44234</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11">
       <c r="A14" s="1">
         <v>44235</v>
       </c>
@@ -1569,7 +1927,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11">
       <c r="A15" s="1">
         <v>44236</v>
       </c>
@@ -1577,7 +1935,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11">
       <c r="A16" s="1">
         <v>44237</v>
       </c>
@@ -1585,152 +1943,657 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:3">
       <c r="A17" s="1">
         <v>44238</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="1">
         <v>44239</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="1">
         <v>44240</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:3">
       <c r="A20" s="1">
         <v>44241</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:3">
       <c r="A21" s="1">
         <v>44242</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="1">
         <v>44243</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="B22" s="4">
+        <v>51</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="1">
         <v>44244</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B23" s="4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="1">
         <v>44245</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="B24" s="4">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="1">
         <v>44246</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="B25" s="4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="1">
         <v>44247</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:3">
       <c r="A27" s="1">
         <v>44248</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:3">
       <c r="A28" s="1">
         <v>44249</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="B28" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="1">
         <v>44250</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="B29" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="1">
         <v>44251</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="B30" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="1">
         <v>44252</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="B31" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="1">
         <v>44253</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="B32" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="1">
         <v>44254</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:3">
       <c r="A34" s="1">
         <v>44255</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:3">
       <c r="A35" s="1">
         <v>44256</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:3">
       <c r="A36" s="1">
         <v>44257</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
+      <c r="B36" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="1">
         <v>44258</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="B37" s="4">
+        <v>49</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="1">
         <v>44259</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
+      <c r="B38" s="4">
+        <v>38</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" s="1">
         <v>44260</v>
       </c>
-    </row>
-    <row r="40" spans="1:1">
+      <c r="B39" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" s="1">
         <v>44261</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:3">
       <c r="A41" s="1">
         <v>44262</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:3">
       <c r="A42" s="1">
         <v>44263</v>
       </c>
+      <c r="B42" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="1">
+        <v>44264</v>
+      </c>
+      <c r="B43" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1">
+        <v>44265</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1">
+        <v>44266</v>
+      </c>
+      <c r="B45" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="1">
+        <v>44267</v>
+      </c>
+      <c r="B46" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="1">
+        <v>44268</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="1">
+        <v>44269</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="1">
+        <v>44270</v>
+      </c>
+      <c r="B49" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="1">
+        <v>44271</v>
+      </c>
+      <c r="B50" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="1">
+        <v>44272</v>
+      </c>
+      <c r="B51" s="4">
+        <v>55</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="1">
+        <v>44273</v>
+      </c>
+      <c r="B52" s="4">
+        <v>55</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="1">
+        <v>44274</v>
+      </c>
+      <c r="B53" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="1">
+        <v>44275</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="1">
+        <v>44276</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="1">
+        <v>44277</v>
+      </c>
+      <c r="B56" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="1">
+        <v>44278</v>
+      </c>
+      <c r="B57" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="1">
+        <v>44279</v>
+      </c>
+      <c r="B58" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="1">
+        <v>44280</v>
+      </c>
+      <c r="B59" s="4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="1">
+        <v>44281</v>
+      </c>
+      <c r="B60" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="1">
+        <v>44282</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="1">
+        <v>44283</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="1">
+        <v>44284</v>
+      </c>
+      <c r="B63" s="4">
+        <v>55</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="1">
+        <v>44285</v>
+      </c>
+      <c r="B64" s="4">
+        <v>55</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1">
+        <v>44286</v>
+      </c>
+      <c r="B65" s="4">
+        <v>55</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B66" s="4">
+        <v>52</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="1">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="1">
+        <v>44289</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="1">
+        <v>44290</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="1">
+        <v>44291</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="1">
+        <v>44292</v>
+      </c>
+      <c r="B71" s="4">
+        <v>55</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="1">
+        <v>44293</v>
+      </c>
+      <c r="B72" s="4">
+        <v>55</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="1">
+        <v>44294</v>
+      </c>
+      <c r="B73" s="4">
+        <v>55</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="1">
+        <v>44295</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="1">
+        <v>44296</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="1">
+        <v>44297</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="1">
+        <v>44298</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="1">
+        <v>44299</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="1">
+        <v>44300</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="1">
+        <v>44301</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="1">
+        <v>44302</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="1">
+        <v>44303</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="1">
+        <v>44304</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="1">
+        <v>44305</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="1">
+        <v>44306</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="1">
+        <v>44307</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="1">
+        <v>44308</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="1">
+        <v>44309</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="1">
+        <v>44310</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="1">
+        <v>44311</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="1">
+        <v>44312</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="1">
+        <v>44313</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="1">
+        <v>44314</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" s="1">
+        <v>44315</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" s="1">
+        <v>44316</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="1">
+        <v>44317</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="1">
+        <v>44318</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="1">
+        <v>44319</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="1">
+        <v>44320</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="1">
+        <v>44321</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="1">
+        <v>44322</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="1">
+        <v>44323</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="1">
+        <v>44324</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="1">
+        <v>44325</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="1">
+        <v>44326</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="1">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="1">
+        <v>44328</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="1">
+        <v>44329</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="1">
+        <v>44330</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="1">
+        <v>44331</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="1">
+        <v>44332</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="1">
+        <v>44333</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>WEEKDAY($A1,2)&gt;=6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="6" priority="4">
+  <conditionalFormatting sqref="B1:B69 B71:B1048576">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
+      <formula>1</formula>
+      <formula>47</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>$B1 &gt; 54</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="5">
       <formula>$B1 &lt; 55</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3">
-      <formula>$B1 &gt; 54</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="between">
-      <formula>1</formula>
-      <formula>47</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C69 C71:C1048576">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$C1 = "not seen!"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
diagram with several input data columns
</commit_message>
<xml_diff>
--- a/cheatsheets/xlsx/formulas.xlsx
+++ b/cheatsheets/xlsx/formulas.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12465"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="21" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>mean:</t>
   </si>
@@ -59,16 +59,13 @@
     <t>not seen!</t>
   </si>
   <si>
-    <t>seen: 44</t>
+    <t>Date</t>
   </si>
   <si>
-    <t>seen: 40</t>
+    <t>Arrived</t>
   </si>
   <si>
-    <t>seen: 42</t>
-  </si>
-  <si>
-    <t>seen: 37</t>
+    <t>Met</t>
   </si>
 </sst>
 </file>
@@ -123,7 +120,39 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -190,8 +219,402 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'21'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Arrived</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'21'!$A$2:$A$81</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="80"/>
+                <c:pt idx="0">
+                  <c:v>44222</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44223</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44224</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44225</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44226</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44227</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44229</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44230</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44231</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44232</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44233</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44234</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44235</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44236</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44237</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44238</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44239</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44240</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44241</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44242</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44243</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44244</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>44245</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44246</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>44247</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44248</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>44249</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>44250</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44251</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44252</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44253</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44254</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44255</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44256</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>44257</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44258</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44259</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>44260</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44261</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44262</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>44263</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44264</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44265</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44266</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44267</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>44268</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>44269</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>44270</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>44271</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>44272</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>44273</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44274</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>44275</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>44276</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>44277</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>44278</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>44279</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>44280</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>44281</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>44282</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>44283</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>44284</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>44285</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>44286</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>44287</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>44288</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>44289</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>44290</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>44291</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>44292</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>44293</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>44294</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>44295</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>44296</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>44297</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>44298</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>44299</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>44300</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>44301</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'21'!$C$2:$C$81</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="80"/>
+                <c:pt idx="62">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-410D-4FBA-8B11-BE7E3DDF6B48}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'21'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Met</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="31750" cap="rnd">
               <a:solidFill>
@@ -284,7 +707,7 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$A$1:$A$80</c:f>
+              <c:f>'21'!$A$2:$A$81</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="80"/>
@@ -533,7 +956,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$1:$B$80</c:f>
+              <c:f>'21'!$B$2:$B$81</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="80"/>
@@ -664,10 +1087,10 @@
                   <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>55</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>55</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="64">
                   <c:v>55</c:v>
@@ -683,6 +1106,12 @@
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>53</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1477,16 +1906,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>695325</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>495301</xdr:colOff>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>38101</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>66676</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1771,829 +2200,858 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K112"/>
+  <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="28" topLeftCell="C62" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="29" topLeftCell="C72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
-      <selection pane="bottomRight" activeCell="B74" sqref="B74"/>
+      <selection pane="bottomRight" activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="11" style="4"/>
-    <col min="3" max="3" width="11" style="6"/>
-    <col min="5" max="5" width="17.875" customWidth="1"/>
+    <col min="2" max="3" width="11" style="4"/>
+    <col min="4" max="4" width="11" style="6"/>
+    <col min="6" max="6" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="1">
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="1">
         <v>44222</v>
       </c>
-      <c r="B1" s="4">
+      <c r="B2" s="4">
         <v>44</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="2">
+      <c r="G2" s="2">
         <f>AVERAGE(B:B)</f>
-        <v>52.591836734693878</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="1">
+        <v>52.666666666666664</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1">
         <v>44223</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B3" s="4">
         <v>50</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G3" s="2">
         <f>(COUNTIF(B:B,"&lt;55")/COUNT(B:B))*100</f>
-        <v>34.693877551020407</v>
-      </c>
-      <c r="G2" s="5"/>
-      <c r="K2">
+        <v>37.254901960784316</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="L3">
         <f>IF(B:B &lt; 55,1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="1">
+    <row r="4" spans="1:12">
+      <c r="A4" s="1">
         <v>44224</v>
       </c>
-      <c r="B3" s="4">
-        <v>55</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="B4" s="4">
+        <v>55</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F3">
+      <c r="G4">
         <f>COUNT(B:B)</f>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="1">
         <v>44225</v>
       </c>
-      <c r="B4" s="4">
-        <v>55</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="B5" s="4">
+        <v>55</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F4">
+      <c r="G5">
         <f>COUNTIF(B:B,"&lt;55")</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="1">
         <v>44226</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F5">
+      <c r="G6">
         <f>COUNTIF(B:B,"&gt;54")</f>
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="1">
+    <row r="7" spans="1:12">
+      <c r="A7" s="1">
         <v>44227</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="1">
+    <row r="8" spans="1:12">
+      <c r="A8" s="1">
         <v>44228</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B8" s="4">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="1">
+    <row r="9" spans="1:12">
+      <c r="A9" s="1">
         <v>44229</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B9" s="4">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="1">
+    <row r="10" spans="1:12">
+      <c r="A10" s="1">
         <v>44230</v>
       </c>
-      <c r="B9" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="1">
+      <c r="B10" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="1">
         <v>44231</v>
       </c>
-      <c r="B10" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="1">
+      <c r="B11" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="1">
         <v>44232</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B12" s="4">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="1">
+    <row r="13" spans="1:12">
+      <c r="A13" s="1">
         <v>44233</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="1">
+    <row r="14" spans="1:12">
+      <c r="A14" s="1">
         <v>44234</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="1">
+    <row r="15" spans="1:12">
+      <c r="A15" s="1">
         <v>44235</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B15" s="4">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="1">
+    <row r="16" spans="1:12">
+      <c r="A16" s="1">
         <v>44236</v>
       </c>
-      <c r="B15" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="1">
+      <c r="B16" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
         <v>44237</v>
       </c>
-      <c r="B16" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1">
+      <c r="B17" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1">
         <v>44238</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B18" s="4">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1">
+    <row r="19" spans="1:4">
+      <c r="A19" s="1">
         <v>44239</v>
       </c>
-      <c r="B18" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1">
+      <c r="B19" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1">
         <v>44240</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1">
+    <row r="21" spans="1:4">
+      <c r="A21" s="1">
         <v>44241</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1">
+    <row r="22" spans="1:4">
+      <c r="A22" s="1">
         <v>44242</v>
       </c>
-      <c r="B21" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="1">
+      <c r="B22" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1">
         <v>44243</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B23" s="4">
         <v>51</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="1">
+    <row r="24" spans="1:4">
+      <c r="A24" s="1">
         <v>44244</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B24" s="4">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="1">
+    <row r="25" spans="1:4">
+      <c r="A25" s="1">
         <v>44245</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B25" s="4">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="1">
+    <row r="26" spans="1:4">
+      <c r="A26" s="1">
         <v>44246</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B26" s="4">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="1">
+    <row r="27" spans="1:4">
+      <c r="A27" s="1">
         <v>44247</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="1">
+    <row r="28" spans="1:4">
+      <c r="A28" s="1">
         <v>44248</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="1">
+    <row r="29" spans="1:4">
+      <c r="A29" s="1">
         <v>44249</v>
       </c>
-      <c r="B28" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="1">
+      <c r="B29" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1">
         <v>44250</v>
       </c>
-      <c r="B29" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="1">
+      <c r="B30" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1">
         <v>44251</v>
       </c>
-      <c r="B30" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="1">
+      <c r="B31" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1">
         <v>44252</v>
-      </c>
-      <c r="B31" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="1">
-        <v>44253</v>
       </c>
       <c r="B32" s="4">
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:4">
       <c r="A33" s="1">
+        <v>44253</v>
+      </c>
+      <c r="B33" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1">
         <v>44254</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="1">
+    <row r="35" spans="1:4">
+      <c r="A35" s="1">
         <v>44255</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="1">
+    <row r="36" spans="1:4">
+      <c r="A36" s="1">
         <v>44256</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="1">
+    <row r="37" spans="1:4">
+      <c r="A37" s="1">
         <v>44257</v>
       </c>
-      <c r="B36" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="1">
+      <c r="B37" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1">
         <v>44258</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B38" s="4">
         <v>49</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="D38" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="1">
+    <row r="39" spans="1:4">
+      <c r="A39" s="1">
         <v>44259</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B39" s="4">
         <v>38</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="D39" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="1">
+    <row r="40" spans="1:4">
+      <c r="A40" s="1">
         <v>44260</v>
       </c>
-      <c r="B39" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="1">
+      <c r="B40" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1">
         <v>44261</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="1">
+    <row r="42" spans="1:4">
+      <c r="A42" s="1">
         <v>44262</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="1">
+    <row r="43" spans="1:4">
+      <c r="A43" s="1">
         <v>44263</v>
       </c>
-      <c r="B42" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="1">
+      <c r="B43" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1">
         <v>44264</v>
       </c>
-      <c r="B43" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="1">
+      <c r="B44" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1">
         <v>44265</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="D45" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="1">
+    <row r="46" spans="1:4">
+      <c r="A46" s="1">
         <v>44266</v>
       </c>
-      <c r="B45" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="1">
+      <c r="B46" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1">
         <v>44267</v>
       </c>
-      <c r="B46" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="1">
+      <c r="B47" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1">
         <v>44268</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="1">
+    <row r="49" spans="1:4">
+      <c r="A49" s="1">
         <v>44269</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="1">
+    <row r="50" spans="1:4">
+      <c r="A50" s="1">
         <v>44270</v>
       </c>
-      <c r="B49" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="1">
+      <c r="B50" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="1">
         <v>44271</v>
       </c>
-      <c r="B50" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="1">
+      <c r="B51" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="1">
         <v>44272</v>
       </c>
-      <c r="B51" s="4">
-        <v>55</v>
-      </c>
-      <c r="C51" s="7" t="s">
+      <c r="B52" s="4">
+        <v>55</v>
+      </c>
+      <c r="D52" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="1">
+    <row r="53" spans="1:4">
+      <c r="A53" s="1">
         <v>44273</v>
       </c>
-      <c r="B52" s="4">
-        <v>55</v>
-      </c>
-      <c r="C52" s="7" t="s">
+      <c r="B53" s="4">
+        <v>55</v>
+      </c>
+      <c r="D53" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="1">
+    <row r="54" spans="1:4">
+      <c r="A54" s="1">
         <v>44274</v>
       </c>
-      <c r="B53" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="1">
+      <c r="B54" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="1">
         <v>44275</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="1">
+    <row r="56" spans="1:4">
+      <c r="A56" s="1">
         <v>44276</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="1">
+    <row r="57" spans="1:4">
+      <c r="A57" s="1">
         <v>44277</v>
       </c>
-      <c r="B56" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="1">
+      <c r="B57" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="1">
         <v>44278</v>
       </c>
-      <c r="B57" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="1">
+      <c r="B58" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="1">
         <v>44279</v>
       </c>
-      <c r="B58" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="1">
+      <c r="B59" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="1">
         <v>44280</v>
       </c>
-      <c r="B59" s="4">
+      <c r="B60" s="4">
         <v>36</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="1">
+    <row r="61" spans="1:4">
+      <c r="A61" s="1">
         <v>44281</v>
       </c>
-      <c r="B60" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="1">
+      <c r="B61" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="1">
         <v>44282</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="1">
+    <row r="63" spans="1:4">
+      <c r="A63" s="1">
         <v>44283</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="1">
+    <row r="64" spans="1:4">
+      <c r="A64" s="1">
         <v>44284</v>
       </c>
-      <c r="B63" s="4">
-        <v>55</v>
-      </c>
-      <c r="C63" s="6" t="s">
+      <c r="B64" s="4">
+        <v>56</v>
+      </c>
+      <c r="C64" s="4">
+        <v>55</v>
+      </c>
+      <c r="D64" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="1">
+    <row r="65" spans="1:4">
+      <c r="A65" s="1">
         <v>44285</v>
       </c>
-      <c r="B64" s="4">
-        <v>55</v>
-      </c>
-      <c r="C64" s="6" t="s">
+      <c r="B65" s="4">
+        <v>56</v>
+      </c>
+      <c r="C65" s="4">
+        <v>55</v>
+      </c>
+      <c r="D65" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="1">
+    <row r="66" spans="1:4">
+      <c r="A66" s="1">
         <v>44286</v>
       </c>
-      <c r="B65" s="4">
-        <v>55</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="1">
+      <c r="B66" s="4">
+        <v>55</v>
+      </c>
+      <c r="C66" s="4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="1">
         <v>44287</v>
       </c>
-      <c r="B66" s="4">
+      <c r="B67" s="4">
         <v>52</v>
       </c>
-      <c r="C66" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="1">
+      <c r="C67" s="4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="1">
         <v>44288</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="1">
+    <row r="69" spans="1:4">
+      <c r="A69" s="1">
         <v>44289</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="1">
+    <row r="70" spans="1:4">
+      <c r="A70" s="1">
         <v>44290</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="1">
+    <row r="71" spans="1:4">
+      <c r="A71" s="1">
         <v>44291</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="1">
+    <row r="72" spans="1:4">
+      <c r="A72" s="1">
         <v>44292</v>
       </c>
-      <c r="B71" s="4">
-        <v>55</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="1">
+      <c r="B72" s="4">
+        <v>55</v>
+      </c>
+      <c r="C72" s="4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="1">
         <v>44293</v>
       </c>
-      <c r="B72" s="4">
-        <v>55</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="1">
+      <c r="B73" s="4">
+        <v>55</v>
+      </c>
+      <c r="C73" s="4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="1">
         <v>44294</v>
       </c>
-      <c r="B73" s="4">
-        <v>55</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="1">
+      <c r="B74" s="4">
+        <v>55</v>
+      </c>
+      <c r="C74" s="4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="1">
         <v>44295</v>
       </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="1">
+      <c r="B75" s="4">
+        <v>54</v>
+      </c>
+      <c r="C75" s="4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="1">
         <v>44296</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="1">
+    <row r="77" spans="1:4">
+      <c r="A77" s="1">
         <v>44297</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="1">
+    <row r="78" spans="1:4">
+      <c r="A78" s="1">
         <v>44298</v>
       </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" s="1">
+      <c r="B78" s="4">
+        <v>53</v>
+      </c>
+      <c r="C78" s="4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="1">
         <v>44299</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="1">
+    <row r="80" spans="1:4">
+      <c r="A80" s="1">
         <v>44300</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="1">
-        <v>44301</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="1">
-        <v>44302</v>
+        <v>44301</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="1">
-        <v>44303</v>
+        <v>44302</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" s="1">
-        <v>44304</v>
+        <v>44303</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" s="1">
-        <v>44305</v>
+        <v>44304</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" s="1">
-        <v>44306</v>
+        <v>44305</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" s="1">
-        <v>44307</v>
+        <v>44306</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" s="1">
-        <v>44308</v>
+        <v>44307</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="1">
-        <v>44309</v>
+        <v>44308</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" s="1">
-        <v>44310</v>
+        <v>44309</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="1">
-        <v>44311</v>
+        <v>44310</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" s="1">
-        <v>44312</v>
+        <v>44311</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" s="1">
-        <v>44313</v>
+        <v>44312</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" s="1">
-        <v>44314</v>
+        <v>44313</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" s="1">
-        <v>44315</v>
+        <v>44314</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" s="1">
-        <v>44316</v>
+        <v>44315</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" s="1">
-        <v>44317</v>
+        <v>44316</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" s="1">
-        <v>44318</v>
+        <v>44317</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" s="1">
-        <v>44319</v>
+        <v>44318</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" s="1">
-        <v>44320</v>
+        <v>44319</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" s="1">
-        <v>44321</v>
+        <v>44320</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" s="1">
-        <v>44322</v>
+        <v>44321</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" s="1">
-        <v>44323</v>
+        <v>44322</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" s="1">
-        <v>44324</v>
+        <v>44323</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" s="1">
-        <v>44325</v>
+        <v>44324</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" s="1">
-        <v>44326</v>
+        <v>44325</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" s="1">
-        <v>44327</v>
+        <v>44326</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" s="1">
-        <v>44328</v>
+        <v>44327</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" s="1">
-        <v>44329</v>
+        <v>44328</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" s="1">
-        <v>44330</v>
+        <v>44329</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" s="1">
-        <v>44331</v>
+        <v>44330</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" s="1">
-        <v>44332</v>
+        <v>44331</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" s="1">
+        <v>44332</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="1">
         <v>44333</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="expression" dxfId="4" priority="8">
-      <formula>WEEKDAY($A1,2)&gt;=6</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B69 B71:B1048576">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
+  <conditionalFormatting sqref="B2:B70 B72:B1048576">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
       <formula>1</formula>
       <formula>47</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>$B1 &gt; 54</formula>
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>$B2 &gt; 54</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="5">
-      <formula>$B1 &lt; 55</formula>
+    <cfRule type="expression" dxfId="2" priority="5">
+      <formula>$B2 &lt; 55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C69 C71:C1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$C1 = "not seen!"</formula>
+  <conditionalFormatting sqref="D2:D70 D72:D1048576">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$D2 = "not seen!"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="expression" dxfId="0" priority="9">
+      <formula>WEEKDAY($A2,2)&gt;=6</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>